<commit_message>
Fix points with same results
</commit_message>
<xml_diff>
--- a/results_2.xlsx
+++ b/results_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="18">
   <si>
     <t>grid_size</t>
   </si>
@@ -93,10 +93,7 @@
     <t>(Alle)</t>
   </si>
   <si>
-    <t>Summe von true_cov</t>
-  </si>
-  <si>
-    <t>Summe von est_cov</t>
+    <t>Summe von difference</t>
   </si>
 </sst>
 </file>
@@ -645,6 +642,1262 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[results_2.xlsx]Tabelle1!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="34925" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="34925" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="34925" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="34925" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ergebnis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$A$7:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$7:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.7017263466949799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1079217972532582</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4102411921507101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-79D5-4A13-8545-66C3116C0211}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="142567344"/>
+        <c:axId val="142561104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="142567344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="142561104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="142561104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="142567344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -688,7 +1941,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4686300" y="368300"/>
+              <a:off x="4762500" y="368300"/>
               <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -760,7 +2013,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6616700" y="406400"/>
+              <a:off x="6692900" y="406400"/>
               <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -832,7 +2085,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8686800" y="425450"/>
+              <a:off x="8763000" y="425450"/>
               <a:ext cx="1828800" cy="2524125"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -861,6 +2114,36 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3359,8 +4642,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A6:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A6:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -3400,9 +4683,9 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -3421,16 +4704,8 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <pageFields count="4">
     <pageField fld="2" item="2" hier="-1"/>
@@ -3438,9 +4713,8 @@
     <pageField fld="3" item="2" hier="-1"/>
     <pageField fld="4" item="0" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Summe von true_cov" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Summe von est_cov" fld="6" baseField="0" baseItem="0"/>
+  <dataFields count="1">
+    <dataField name="Summe von difference" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3773,20 +5047,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3794,7 +5068,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3802,7 +5076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3810,7 +5084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3818,59 +5092,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>30</v>
       </c>
       <c r="B7" s="3">
-        <v>2.0596669432073322</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.35794059651235222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1.7017263466949799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>50</v>
       </c>
       <c r="B8" s="3">
-        <v>2.4018476876051471</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.29392589035189048</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2.1079217972532582</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>70</v>
       </c>
       <c r="B9" s="3">
-        <v>2.565090172516685</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.15484898036597422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2.4102411921507101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>7.0266048033291639</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.80671546723021703</v>
+        <v>6.219889336098948</v>
       </c>
     </row>
   </sheetData>
@@ -10525,16 +11784,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8C50234-C519-4C88-B1FA-178063CCCDA7}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="0b08a281-9514-415a-a874-508dd73fb2f6"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0b08a281-9514-415a-a874-508dd73fb2f6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="5f8c50f4-1dc1-407f-9f16-a75853b3c174"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>